<commit_message>
Calcular costo social solo un empleado marinos
</commit_message>
<xml_diff>
--- a/XurtepNominas/bin/Debug/Archivos/nominasmarinos.xlsx
+++ b/XurtepNominas/bin/Debug/Archivos/nominasmarinos.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
   <si>
     <t>TRABAJADOR</t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>3 % S/NÓM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t>COSTO SOCIAL REAL</t>
   </si>
 </sst>
 </file>
@@ -2017,20 +2026,20 @@
     <xf numFmtId="43" fontId="37" fillId="0" borderId="0" xfId="797" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="61" fillId="0" borderId="0" xfId="798" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="61" fillId="0" borderId="0" xfId="797" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2903,7 +2912,7 @@
         <xdr:cNvPr id="3" name="2 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2982,7 +2991,7 @@
         <xdr:cNvPr id="3" name="2 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3061,7 +3070,7 @@
         <xdr:cNvPr id="2" name="1 Imagen">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4295,152 +4304,152 @@
       <c r="AI8" s="1"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="K9" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="56" t="s">
+      <c r="M9" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="56" t="s">
+      <c r="O9" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="P9" s="56" t="s">
+      <c r="P9" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="Q9" s="56" t="s">
+      <c r="Q9" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="R9" s="59" t="s">
+      <c r="R9" s="58" t="s">
         <v>40</v>
       </c>
       <c r="S9" s="31"/>
-      <c r="T9" s="56" t="s">
+      <c r="T9" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="56" t="s">
+      <c r="U9" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="V9" s="56" t="s">
+      <c r="V9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="W9" s="56"/>
-      <c r="X9" s="56" t="s">
+      <c r="W9" s="57"/>
+      <c r="X9" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="Y9" s="56" t="s">
+      <c r="Y9" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="Z9" s="56" t="s">
+      <c r="Z9" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="AA9" s="60" t="s">
+      <c r="AA9" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="AB9" s="60" t="s">
+      <c r="AB9" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="AC9" s="60" t="s">
+      <c r="AC9" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="AD9" s="60" t="s">
+      <c r="AD9" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="AE9" s="60" t="s">
+      <c r="AE9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AF9" s="56" t="s">
+      <c r="AF9" s="57" t="s">
         <v>1</v>
       </c>
       <c r="AG9" s="33"/>
       <c r="AH9" s="33"/>
-      <c r="AI9" s="56" t="s">
+      <c r="AI9" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="AK9" s="57" t="s">
+      <c r="AK9" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="AL9" s="58" t="s">
+      <c r="AL9" s="60" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="59"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="58"/>
       <c r="S10" s="31"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
-      <c r="X10" s="56"/>
-      <c r="Y10" s="56"/>
-      <c r="Z10" s="56"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="56"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="56"/>
+      <c r="AB10" s="56"/>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
+      <c r="AF10" s="57"/>
       <c r="AG10" s="32" t="s">
         <v>2</v>
       </c>
       <c r="AH10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="AI10" s="56"/>
-      <c r="AK10" s="57"/>
-      <c r="AL10" s="58"/>
+      <c r="AI10" s="57"/>
+      <c r="AK10" s="59"/>
+      <c r="AL10" s="60"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="F11" s="30"/>
@@ -4575,24 +4584,6 @@
     <sortCondition ref="C11:C23"/>
   </sortState>
   <mergeCells count="34">
-    <mergeCell ref="AA9:AA10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="J9:J10"/>
     <mergeCell ref="T9:T10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="AK9:AK10"/>
@@ -4609,6 +4600,24 @@
     <mergeCell ref="Z9:Z10"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="AA9:AA10"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AB9:AB10"/>
+    <mergeCell ref="AE9:AE10"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
@@ -4619,13 +4628,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:AL12"/>
+  <dimension ref="A1:AS12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane xSplit="1" ySplit="11" topLeftCell="T12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="AG11" sqref="AG11"/>
+      <selection pane="bottomRight" activeCell="AN11" sqref="AN11:AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4658,7 +4667,7 @@
     <col min="38" max="38" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="44"/>
       <c r="B1" s="61" t="s">
         <v>31</v>
@@ -4682,7 +4691,7 @@
       <c r="AK1" s="22"/>
       <c r="AL1" s="22"/>
     </row>
-    <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="62" t="s">
         <v>49</v>
@@ -4706,7 +4715,7 @@
       <c r="AK2" s="22"/>
       <c r="AL2" s="22"/>
     </row>
-    <row r="3" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
       <c r="B3" s="63" t="s">
         <v>32</v>
@@ -4731,7 +4740,7 @@
       <c r="AK3" s="22"/>
       <c r="AL3" s="22"/>
     </row>
-    <row r="4" spans="1:38" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
       <c r="B4" s="43"/>
       <c r="C4" s="42"/>
@@ -4773,7 +4782,7 @@
       <c r="AK4" s="22"/>
       <c r="AL4" s="22"/>
     </row>
-    <row r="5" spans="1:38" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
       <c r="B5" s="43"/>
       <c r="C5" s="42"/>
@@ -4813,7 +4822,7 @@
       <c r="AK5" s="22"/>
       <c r="AL5" s="22"/>
     </row>
-    <row r="6" spans="1:38" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="43"/>
       <c r="C6" s="42"/>
@@ -4853,7 +4862,7 @@
       <c r="AK6" s="22"/>
       <c r="AL6" s="22"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="64" t="s">
         <v>82</v>
@@ -4878,7 +4887,7 @@
       <c r="AK7" s="22"/>
       <c r="AL7" s="22"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="11" t="s">
         <v>50</v>
@@ -4902,7 +4911,7 @@
       <c r="AK8" s="22"/>
       <c r="AL8" s="22"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="11" t="s">
         <v>51</v>
@@ -4926,7 +4935,7 @@
       <c r="AK9" s="22"/>
       <c r="AL9" s="22"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -4948,7 +4957,7 @@
       <c r="AK10" s="22"/>
       <c r="AL10" s="22"/>
     </row>
-    <row r="11" spans="1:38" s="8" customFormat="1" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" s="8" customFormat="1" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>36</v>
       </c>
@@ -5063,8 +5072,26 @@
       <c r="AL11" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="AN11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ11" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS11" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A12:AK25">
     <sortCondition ref="B12:B25"/>
@@ -5088,13 +5115,13 @@
   <sheetPr codeName="Hoja8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL13"/>
+  <dimension ref="A1:AS13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="L12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="11" topLeftCell="T12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="AG1" sqref="AG1:AG1048576"/>
+      <selection pane="bottomRight" activeCell="AN11" sqref="AN11:AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5116,10 +5143,12 @@
     <col min="33" max="33" width="11.42578125" style="46" customWidth="1"/>
     <col min="34" max="37" width="11.42578125" style="22" customWidth="1"/>
     <col min="38" max="38" width="12.7109375" style="22" customWidth="1"/>
-    <col min="39" max="16384" width="10.85546875" style="22"/>
+    <col min="39" max="44" width="10.85546875" style="22"/>
+    <col min="45" max="45" width="18.7109375" style="22" customWidth="1"/>
+    <col min="46" max="16384" width="10.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="61" t="s">
         <v>31</v>
@@ -5131,7 +5160,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="62" t="s">
         <v>49</v>
@@ -5143,7 +5172,7 @@
       <c r="G2" s="67"/>
       <c r="H2" s="67"/>
     </row>
-    <row r="3" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="63" t="s">
         <v>32</v>
       </c>
@@ -5155,7 +5184,7 @@
       <c r="H3" s="66"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="37"/>
       <c r="C4" s="36"/>
       <c r="D4" s="65" t="s">
@@ -5167,7 +5196,7 @@
       <c r="H4" s="36"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="37"/>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -5177,7 +5206,7 @@
       <c r="H5" s="36"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="37"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -5187,7 +5216,7 @@
       <c r="H6" s="36"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B7" s="68" t="str">
         <f>'XURTEP ABORDO'!B7:H7</f>
         <v>Periodo  Adicional del 01/09/2018 al 30/09/2018</v>
@@ -5200,7 +5229,7 @@
       <c r="H7" s="68"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>50</v>
       </c>
@@ -5212,15 +5241,15 @@
       <c r="R8" s="19"/>
       <c r="S8" s="19"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="36"/>
     </row>
-    <row r="11" spans="1:38" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>36</v>
       </c>
@@ -5335,9 +5364,27 @@
       <c r="AL11" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ11" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS11" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="AL13" s="23"/>
     </row>
   </sheetData>
@@ -5466,44 +5513,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="57" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D5" s="46"/>

</xml_diff>